<commit_message>
Atualiza dicionário de dados conforme tooltip do Portal
</commit_message>
<xml_diff>
--- a/data-raw/dicionario-dados.xlsx
+++ b/data-raw/dicionario-dados.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fjunior/Local/github/transparencia-mg/dt-contratacoes-coronavirus/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\1.CGE\tele-trabalho\GIT\dt-contratacoes-coronavirus\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834DE620-6867-DB43-A87C-95B1356A3D39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{9A7A9267-65D2-8943-9C0A-E4045745D472}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="21135"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -65,18 +64,6 @@
     <t>PROCEDIMENTO_CONTRATACAO</t>
   </si>
   <si>
-    <t>NUMERO_CONTRATO</t>
-  </si>
-  <si>
-    <t>URL_INTEGRA_CONTRATO</t>
-  </si>
-  <si>
-    <t>CODIGO_ORGAO_CONTRATO</t>
-  </si>
-  <si>
-    <t>ORGAO_CONTRATO</t>
-  </si>
-  <si>
     <t>DATA_PUBLICACAO</t>
   </si>
   <si>
@@ -224,36 +211,12 @@
     <t>Inclui as modalidades de licitação (concorrência, tomada de preços, convite e leilão), pregão, dispensa, inexigibilidade, registro de preços, etc.</t>
   </si>
   <si>
-    <t>Número do contrato no Sistema Integrado de Administração Financeira de Minas Gerais (SIAFI-MG).  Campo opcional, NA em caso de ausência de contratos por serem de entrega imediata.</t>
-  </si>
-  <si>
-    <t>Link para íntegra do termo do contrato celebrado e seus eventuais termos aditivos ou modificativos.</t>
-  </si>
-  <si>
-    <t>Código do órgão ou entidade responsável pelo contrato.</t>
-  </si>
-  <si>
-    <t>Nome do órgão ou entidade responsável pelo contrato</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
     <t>Data, no formato YYYY-MM-DD, de publicação do Contrato no IOF</t>
   </si>
   <si>
-    <t>Data, no formato YYYY-MM-DD, de início da vigência do contrato</t>
-  </si>
-  <si>
-    <t>Data, no formato YYYY-MM-DD, de fim da vigência do contrato</t>
-  </si>
-  <si>
-    <t>Data, no formato YYYY-MM-DD, de fim da vigência do contrato atualizada</t>
-  </si>
-  <si>
-    <t>Número de identificação do fornecedor. Pessoa Jurídica – CNPJ. Pessoa física CPF. Formato: (eg. xx.xxx.xxx/yyyy-zz e xxx.xxx.xxx-zz).</t>
-  </si>
-  <si>
     <t>Nome da pessoa física ou jurídica contratada para prestar um serviço ou entregar bens materiais ao Estado.</t>
   </si>
   <si>
@@ -263,18 +226,6 @@
     <t xml:space="preserve">Link para consulta do processo eletrônico no Sistema Eletrônico de Informações (SEI) </t>
   </si>
   <si>
-    <t>Código do  item de bem ou serviço adquirido pelo Estado.</t>
-  </si>
-  <si>
-    <t>Descrição dos itens de bens ou serviços adquiridos pelo Estado.</t>
-  </si>
-  <si>
-    <t>Código da unidade orçamentária vinculada ao item de pedido de compra</t>
-  </si>
-  <si>
-    <t>Nome da unidade orçamentária vinculada ao item de pedido de compra</t>
-  </si>
-  <si>
     <t>Descrição da linha de fornecimento vinculada ao item material/serviço.</t>
   </si>
   <si>
@@ -348,12 +299,60 @@
   </si>
   <si>
     <t>Cidade Entrega</t>
+  </si>
+  <si>
+    <t>Código do órgão ou entidade que formalizou o instrumento de contratação.</t>
+  </si>
+  <si>
+    <t>Número de identificação do fornecedor. Pessoa Jurídica – CNPJ. Pessoa física - CPF. Formato: (eg. xx.xxx.xxx/yyyy-zz e xxx.xxx.xxx-zz).</t>
+  </si>
+  <si>
+    <t>Código do item de material ou serviço adquirido pelo Estado.</t>
+  </si>
+  <si>
+    <t>Descrição dos itens de materiais ou serviços adquiridos pelo Estado.</t>
+  </si>
+  <si>
+    <t>Código da unidade orçamentária vinculada ao item material/serviço.</t>
+  </si>
+  <si>
+    <t>Nome da Unidade Orçamentária vinculada ao item material/serviço.</t>
+  </si>
+  <si>
+    <t>NUMERO_Contrato</t>
+  </si>
+  <si>
+    <t>Número do Contrato registrado no Sistema Integrado de Administração Financeira de Minas Gerais (SIAFI-MG).  "NA" em caso de ausência de Contratos por serem de entrega imediata.</t>
+  </si>
+  <si>
+    <t>URL_INTEGRA_Contrato</t>
+  </si>
+  <si>
+    <t>Link para íntegra do termo do Contrato celebrado e seus eventuais termos aditivos ou modificativos.</t>
+  </si>
+  <si>
+    <t>CODIGO_ORGAO_Contrato</t>
+  </si>
+  <si>
+    <t>ORGAO_Contrato</t>
+  </si>
+  <si>
+    <t>Nome do órgão ou entidade responsável pelo Contrato</t>
+  </si>
+  <si>
+    <t>Data, no formato YYYY-MM-DD, de início da vigência do Contrato</t>
+  </si>
+  <si>
+    <t>Data, no formato YYYY-MM-DD, de fim da vigência do Contrato</t>
+  </si>
+  <si>
+    <t>Data, no formato YYYY-MM-DD, atualizada do fim da vigência do Contrato</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -819,37 +818,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C10582-576F-B04D-A4FA-0CC79FF651E8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="32.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="87.33203125" customWidth="1"/>
+    <col min="5" max="5" width="87.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -857,16 +858,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -874,16 +875,16 @@
         <v>2</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -891,16 +892,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -908,16 +909,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -925,16 +926,16 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -942,16 +943,16 @@
         <v>6</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -959,16 +960,16 @@
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -976,16 +977,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -993,404 +994,404 @@
         <v>9</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>10</v>
+        <v>95</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>22</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>24</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>26</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>28</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>31</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>